<commit_message>
actualizar archivo Excel REV-18-03-2025 y modificar lista de tareas en todo.txt para reflejar el estado actual de las funcionalidades y mejoras implementadas
</commit_message>
<xml_diff>
--- a/REVs/REV-18-03-2025.xlsx
+++ b/REVs/REV-18-03-2025.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A18:XFD23"/>
@@ -1403,20 +1403,63 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>6XS18316</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B.GREEN OMEGA 3 1000MG 30 CAPS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>